<commit_message>
Aggiornamento schede fino a n.46
</commit_message>
<xml_diff>
--- a/01_preparation/grafici_report.xlsx
+++ b/01_preparation/grafici_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CG14469\Documents\GitHub\report-scenario\01_preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1882EC4D-EC8B-4A51-9AA3-DE42872A52E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13395F3-2313-476E-9A42-EF307FAEBBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-78" yWindow="0" windowWidth="10524" windowHeight="12318" firstSheet="26" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-78" yWindow="0" windowWidth="10524" windowHeight="12318" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10_Italian_GDP_Growth_Rate" sheetId="1" r:id="rId1"/>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6978,8 +6978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection sqref="A1:AA4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9239,7 +9239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -10437,7 +10437,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -20528,7 +20528,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -22208,8 +22208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>